<commit_message>
Queue update and moving working
</commit_message>
<xml_diff>
--- a/Label Printing Plan.xlsx
+++ b/Label Printing Plan.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Manual Entry</t>
   </si>
@@ -98,13 +97,16 @@
   </si>
   <si>
     <t>Printer and Paper Tray</t>
+  </si>
+  <si>
+    <t>+ Buttons</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +118,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -220,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -285,6 +294,8 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +600,7 @@
   <dimension ref="D2:AD10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,7 +663,7 @@
       <c r="P5" t="s">
         <v>12</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5" s="22" t="s">
         <v>7</v>
       </c>
       <c r="V5" t="s">
@@ -678,7 +689,7 @@
       <c r="P6" t="s">
         <v>13</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S6" s="22" t="s">
         <v>8</v>
       </c>
     </row>
@@ -708,9 +719,8 @@
       </c>
     </row>
     <row r="9" spans="4:30" x14ac:dyDescent="0.25">
-      <c r="D9" t="e">
-        <f>+ Buttons</f>
-        <v>#NAME?</v>
+      <c r="D9" s="23" t="s">
+        <v>27</v>
       </c>
       <c r="P9" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Added labelstocks, missing pictures
</commit_message>
<xml_diff>
--- a/Label Printing Plan.xlsx
+++ b/Label Printing Plan.xlsx
@@ -234,68 +234,68 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,70 +600,70 @@
   <dimension ref="D2:AD10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="4:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:30" s="1" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="12" t="s">
+      <c r="H3" s="12"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="13" t="s">
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="14"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="16" t="s">
+      <c r="N3" s="16"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="19" t="s">
+      <c r="Q3" s="19"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="T3" s="20"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="2" t="s">
+      <c r="T3" s="22"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="W3" s="2"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="4" t="s">
+      <c r="W3" s="4"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="4" t="s">
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="6"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="8"/>
     </row>
     <row r="5" spans="4:30" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="P5" t="s">
         <v>12</v>
       </c>
-      <c r="S5" s="22" t="s">
+      <c r="S5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="V5" t="s">
@@ -677,7 +677,7 @@
       <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J6" t="s">
@@ -689,12 +689,12 @@
       <c r="P6" t="s">
         <v>13</v>
       </c>
-      <c r="S6" s="22" t="s">
+      <c r="S6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="4:30" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="J7" t="s">
@@ -703,7 +703,7 @@
       <c r="P7" t="s">
         <v>14</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S7" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -711,7 +711,7 @@
       <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="P8" t="s">
@@ -719,7 +719,7 @@
       </c>
     </row>
     <row r="9" spans="4:30" x14ac:dyDescent="0.25">
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="3" t="s">
         <v>27</v>
       </c>
       <c r="P9" t="s">

</xml_diff>